<commit_message>
Add motors, ESCs and props
Added motors, ESCs and props to main sheet.  Also added second sheet
with details of motor and prop options.
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-60" windowWidth="21840" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
   <si>
     <t>Part</t>
   </si>
@@ -145,6 +146,113 @@
   </si>
   <si>
     <t>http://www.hobbyking.com/hobbyking/store/uh_viewItem.asp?idProduct=16529</t>
+  </si>
+  <si>
+    <t>Turnigy D2836-11</t>
+  </si>
+  <si>
+    <t>Turnigy 30A Plush ESC</t>
+  </si>
+  <si>
+    <t>10x4.5 (4 pc)</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Kv (rpm/v)</t>
+  </si>
+  <si>
+    <t>Weight 
+(g)</t>
+  </si>
+  <si>
+    <t>Max Current 
+(A)</t>
+  </si>
+  <si>
+    <t>Resistance 
+(mh)</t>
+  </si>
+  <si>
+    <t>Max Voltage
+ (V)</t>
+  </si>
+  <si>
+    <t>Power 
+(w)</t>
+  </si>
+  <si>
+    <t>Thrust
+(g)</t>
+  </si>
+  <si>
+    <t>Shaft A (mm)</t>
+  </si>
+  <si>
+    <t>Length B
+(mm)</t>
+  </si>
+  <si>
+    <t>Diameter C
+(mm)</t>
+  </si>
+  <si>
+    <t>Can Length D
+(mm)</t>
+  </si>
+  <si>
+    <t>Total Length E 
+(mm)</t>
+  </si>
+  <si>
+    <t>Turnigy D2830-11</t>
+  </si>
+  <si>
+    <t>Turnigy 2830</t>
+  </si>
+  <si>
+    <t>Turnigy 2836</t>
+  </si>
+  <si>
+    <t>NTM 2830</t>
+  </si>
+  <si>
+    <t>Turnigy D2836-9</t>
+  </si>
+  <si>
+    <t>ESC's and Programming Card</t>
+  </si>
+  <si>
+    <t>Turnigy BESC
+Programming Card</t>
+  </si>
+  <si>
+    <t>Slow Fly Electric Props</t>
+  </si>
+  <si>
+    <t>Amps</t>
+  </si>
+  <si>
+    <t>Watts</t>
+  </si>
+  <si>
+    <t>9x4.7 (4pc)</t>
+  </si>
+  <si>
+    <t>9x6 (5 pc)</t>
+  </si>
+  <si>
+    <t>10x3.8 (5 pc)</t>
+  </si>
+  <si>
+    <t>10x6 (6 pc)</t>
+  </si>
+  <si>
+    <t>11x4.7 (4 pc)</t>
+  </si>
+  <si>
+    <t>ESC Programming Card</t>
   </si>
 </sst>
 </file>
@@ -154,7 +262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,16 +307,63 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -225,8 +380,333 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -234,8 +714,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -247,18 +728,112 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="7" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -586,21 +1161,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.125" customWidth="1"/>
+    <col min="2" max="2" width="39.625" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="6" width="11.1640625" customWidth="1"/>
+    <col min="5" max="6" width="11.125" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="102" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1">
+    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -629,7 +1206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -659,7 +1236,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -689,45 +1266,63 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
       <c r="C4" s="3">
         <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>12.46</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="3"/>
+        <v>74.760000000000005</v>
+      </c>
+      <c r="F4" s="3">
+        <f>(67*6)</f>
+        <v>402</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
       <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
       <c r="C5" s="3">
         <v>6</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>12.95</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="3"/>
+        <v>77.699999999999989</v>
+      </c>
+      <c r="F5" s="3">
+        <f>(25*6)</f>
+        <v>150</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -757,7 +1352,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -776,42 +1371,57 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
       <c r="C8" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2">
-        <v>0</v>
+        <v>3.07</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.14</v>
       </c>
       <c r="F8" s="3"/>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
       <c r="H8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
       <c r="C9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2">
-        <v>0</v>
+        <v>3.79</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.58</v>
       </c>
       <c r="F9" s="3"/>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
       <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -830,7 +1440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -849,7 +1459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>33</v>
       </c>
@@ -879,7 +1489,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -909,7 +1519,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -939,7 +1549,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -969,7 +1579,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="3">
         <v>0</v>
       </c>
@@ -985,23 +1595,31 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
       <c r="C17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2">
-        <v>0</v>
+        <v>6.95</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="3"/>
+        <v>6.95</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
       <c r="H17" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C18" s="3">
         <v>0</v>
       </c>
@@ -1017,7 +1635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C19" s="3">
         <v>0</v>
       </c>
@@ -1033,7 +1651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C20" s="3">
         <v>0</v>
       </c>
@@ -1049,7 +1667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C21" s="3">
         <v>0</v>
       </c>
@@ -1065,23 +1683,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1">
+    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="6">
         <f>SUM(E2:E21)</f>
-        <v>278.33000000000004</v>
+        <v>451.46</v>
       </c>
       <c r="F22" s="7">
         <f>SUM(F2:F21)</f>
-        <v>853</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F23" s="7">
         <f>1500-F22</f>
-        <v>647</v>
+        <v>95</v>
       </c>
       <c r="I23" t="s">
         <v>23</v>
@@ -1089,6 +1707,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3" display="http://www.hobbyking.com/hobbyking/store/__22447__Slow_Fly_Electric_Prop_1045R_SF_RH_Rotation_4_pc_.html"/>
+    <hyperlink ref="B17" r:id="rId4" display="http://www.hobbyking.com/hobbyking/store/uh_viewItem.asp?idProduct=2169"/>
+    <hyperlink ref="B9" r:id="rId5" display="http://www.hobbyking.com/hobbyking/store/__22451__Slow_Fly_Electric_Prop_11x4_7SF_RH_Rotation_4_pc_.html"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1097,4 +1722,510 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12"/>
+      <c r="B1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="18">
+        <v>9.56</v>
+      </c>
+      <c r="C2" s="19">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="19">
+        <v>52</v>
+      </c>
+      <c r="E2" s="19">
+        <v>21</v>
+      </c>
+      <c r="F2" s="19">
+        <v>0</v>
+      </c>
+      <c r="G2" s="19">
+        <v>15</v>
+      </c>
+      <c r="H2" s="19">
+        <v>210</v>
+      </c>
+      <c r="I2" s="19">
+        <v>760</v>
+      </c>
+      <c r="J2" s="19">
+        <v>3.17</v>
+      </c>
+      <c r="K2" s="19">
+        <v>30</v>
+      </c>
+      <c r="L2" s="19">
+        <v>28</v>
+      </c>
+      <c r="M2" s="19">
+        <v>14</v>
+      </c>
+      <c r="N2" s="20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="21">
+        <v>12.42</v>
+      </c>
+      <c r="C3" s="22">
+        <v>750</v>
+      </c>
+      <c r="D3" s="22">
+        <v>67</v>
+      </c>
+      <c r="E3" s="22">
+        <v>20</v>
+      </c>
+      <c r="F3" s="22">
+        <v>0</v>
+      </c>
+      <c r="G3" s="22">
+        <v>11</v>
+      </c>
+      <c r="H3" s="22">
+        <v>206</v>
+      </c>
+      <c r="I3" s="22">
+        <v>800</v>
+      </c>
+      <c r="J3" s="22">
+        <v>4</v>
+      </c>
+      <c r="K3" s="22">
+        <v>35</v>
+      </c>
+      <c r="L3" s="22">
+        <v>28</v>
+      </c>
+      <c r="M3" s="22">
+        <v>20</v>
+      </c>
+      <c r="N3" s="23">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="25">
+        <v>14.26</v>
+      </c>
+      <c r="C4" s="26">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="26">
+        <v>54</v>
+      </c>
+      <c r="E4" s="26">
+        <v>18</v>
+      </c>
+      <c r="F4" s="26">
+        <v>0</v>
+      </c>
+      <c r="G4" s="26">
+        <v>11</v>
+      </c>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26">
+        <v>900</v>
+      </c>
+      <c r="J4" s="26">
+        <v>3</v>
+      </c>
+      <c r="K4" s="26">
+        <v>32</v>
+      </c>
+      <c r="L4" s="26">
+        <v>28</v>
+      </c>
+      <c r="M4" s="26">
+        <v>15</v>
+      </c>
+      <c r="N4" s="27">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="25">
+        <v>14.26</v>
+      </c>
+      <c r="C5" s="26">
+        <v>800</v>
+      </c>
+      <c r="D5" s="26">
+        <v>54</v>
+      </c>
+      <c r="E5" s="26">
+        <v>14</v>
+      </c>
+      <c r="F5" s="26">
+        <v>0</v>
+      </c>
+      <c r="G5" s="26">
+        <v>11</v>
+      </c>
+      <c r="H5" s="26">
+        <v>160</v>
+      </c>
+      <c r="I5" s="26">
+        <v>800</v>
+      </c>
+      <c r="J5" s="26">
+        <v>3</v>
+      </c>
+      <c r="K5" s="26">
+        <v>32</v>
+      </c>
+      <c r="L5" s="26">
+        <v>28</v>
+      </c>
+      <c r="M5" s="26">
+        <v>15</v>
+      </c>
+      <c r="N5" s="27">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="25">
+        <v>18.68</v>
+      </c>
+      <c r="C6" s="26">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="26">
+        <v>80</v>
+      </c>
+      <c r="E6" s="26">
+        <v>27</v>
+      </c>
+      <c r="F6" s="26">
+        <v>0</v>
+      </c>
+      <c r="G6" s="26">
+        <v>11</v>
+      </c>
+      <c r="H6" s="26">
+        <v>300</v>
+      </c>
+      <c r="I6" s="26">
+        <v>1000</v>
+      </c>
+      <c r="J6" s="26">
+        <v>4</v>
+      </c>
+      <c r="K6" s="26">
+        <v>37</v>
+      </c>
+      <c r="L6" s="26">
+        <v>28</v>
+      </c>
+      <c r="M6" s="26">
+        <v>22</v>
+      </c>
+      <c r="N6" s="27">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="25">
+        <v>14.99</v>
+      </c>
+      <c r="C7" s="26">
+        <v>750</v>
+      </c>
+      <c r="D7" s="26">
+        <v>67</v>
+      </c>
+      <c r="E7" s="26">
+        <v>20</v>
+      </c>
+      <c r="F7" s="26">
+        <v>0</v>
+      </c>
+      <c r="G7" s="26">
+        <v>15</v>
+      </c>
+      <c r="H7" s="26">
+        <v>140</v>
+      </c>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26">
+        <v>3</v>
+      </c>
+      <c r="K7" s="26">
+        <v>32</v>
+      </c>
+      <c r="L7" s="26">
+        <v>28</v>
+      </c>
+      <c r="M7" s="26">
+        <v>19</v>
+      </c>
+      <c r="N7" s="27">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="29">
+        <v>12.22</v>
+      </c>
+      <c r="C8" s="30">
+        <v>950</v>
+      </c>
+      <c r="D8" s="30">
+        <v>70</v>
+      </c>
+      <c r="E8" s="30">
+        <v>23</v>
+      </c>
+      <c r="F8" s="30">
+        <v>0</v>
+      </c>
+      <c r="G8" s="30">
+        <v>15</v>
+      </c>
+      <c r="H8" s="30">
+        <v>243</v>
+      </c>
+      <c r="I8" s="30">
+        <v>850</v>
+      </c>
+      <c r="J8" s="30">
+        <v>4</v>
+      </c>
+      <c r="K8" s="30">
+        <v>30</v>
+      </c>
+      <c r="L8" s="30">
+        <v>28</v>
+      </c>
+      <c r="M8" s="30">
+        <v>19</v>
+      </c>
+      <c r="N8" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="54"/>
+    </row>
+    <row r="12" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="33">
+        <v>12.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="35">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="37">
+        <v>3.02</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="40"/>
+    </row>
+    <row r="18" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="42">
+        <v>2.69</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="45"/>
+    </row>
+    <row r="19" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="42">
+        <v>3.36</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="45"/>
+    </row>
+    <row r="20" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="46">
+        <v>3.07</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47">
+        <v>9.5</v>
+      </c>
+      <c r="F20" s="48">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="42">
+        <v>3.48</v>
+      </c>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44">
+        <v>11</v>
+      </c>
+      <c r="F21" s="50">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="52">
+        <v>3.79</v>
+      </c>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53">
+        <v>12</v>
+      </c>
+      <c r="F22" s="35">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:B11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="A8" r:id="rId6"/>
+    <hyperlink ref="A3" r:id="rId7"/>
+    <hyperlink ref="A13" r:id="rId8" display="http://www.hobbyking.com/hobbyking/store/uh_viewItem.asp?idProduct=2169"/>
+    <hyperlink ref="A12" r:id="rId9"/>
+    <hyperlink ref="A20" r:id="rId10" display="http://www.hobbyking.com/hobbyking/store/__22447__Slow_Fly_Electric_Prop_1045R_SF_RH_Rotation_4_pc_.html"/>
+    <hyperlink ref="A22" r:id="rId11" display="http://www.hobbyking.com/hobbyking/store/__22451__Slow_Fly_Electric_Prop_11x4_7SF_RH_Rotation_4_pc_.html"/>
+    <hyperlink ref="A17" r:id="rId12"/>
+    <hyperlink ref="A21" r:id="rId13"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Initial Parts Ordered. Updated with part info and order status
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-60" windowWidth="21840" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28320" windowHeight="14980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>Part</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Battery (Main)</t>
   </si>
   <si>
-    <t>Battery (Control)</t>
-  </si>
-  <si>
     <t>Props</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
   </si>
   <si>
     <t>Remaining Weight Budget</t>
-  </si>
-  <si>
-    <t>Hooby King</t>
   </si>
   <si>
     <t>http://witespyquad.gostorego.com/multiwii-pro-2-0-flight-controller.html</t>
@@ -253,6 +247,45 @@
   </si>
   <si>
     <t>ESC Programming Card</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>http://www.hobbyking.com/hobbyking/store/__10313__Turnigy_5A_8_40v_SBEC_for_Lipo_.html</t>
+  </si>
+  <si>
+    <t>SBEC</t>
+  </si>
+  <si>
+    <t>Turnigy 5A (8-40v) SBEC for Lipo</t>
+  </si>
+  <si>
+    <t>http://www.hobbyking.com/hobbyking/store/__31223__Hobbyking_Multi_Rotor_Power_Distribution_Board_DIY_8_x_output_PCB_.html</t>
+  </si>
+  <si>
+    <t>Hobbyking Multi-Rotor Power Distribution Board (DIY 8 x output PCB)</t>
+  </si>
+  <si>
+    <t>Shipping 1</t>
+  </si>
+  <si>
+    <t>Onboard Display</t>
+  </si>
+  <si>
+    <t>http://witespyquad.gostorego.com/flight-controllers/3dr-radio-telemetry-kit-915mhz.html</t>
+  </si>
+  <si>
+    <t>3DR Radio Telemetry Kit 915Mhz</t>
+  </si>
+  <si>
+    <t>http://witespyquad.gostorego.com/flight-controllers/readytofly-1-oled-128x64-pid-tuning-display-i2c.html</t>
+  </si>
+  <si>
+    <t>ReadyToFlyQuads 1" OLED Display</t>
+  </si>
+  <si>
+    <t>Telemetry Radio</t>
   </si>
 </sst>
 </file>
@@ -382,331 +415,331 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -715,6 +748,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -763,9 +803,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -813,14 +850,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1159,25 +1206,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.125" customWidth="1"/>
-    <col min="2" max="2" width="39.625" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="6" width="11.125" customWidth="1"/>
+    <col min="5" max="6" width="11.1640625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="102" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="5" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1241,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>4</v>
@@ -1206,12 +1253,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -1227,21 +1274,21 @@
         <v>410</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -1250,28 +1297,28 @@
         <v>89</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E21" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E25" si="0">C3*D3</f>
         <v>89</v>
       </c>
       <c r="F3" s="3">
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3">
         <v>6</v>
@@ -1288,46 +1335,43 @@
         <v>402</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
       <c r="C5" s="3">
         <v>6</v>
       </c>
       <c r="D5" s="2">
-        <v>12.95</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>77.699999999999989</v>
+        <v>0</v>
       </c>
       <c r="F5" s="3">
         <f>(25*6)</f>
         <v>150</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -1343,106 +1387,128 @@
         <v>409</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>5.98</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="3"/>
+        <v>5.98</v>
+      </c>
+      <c r="F7" s="3">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
       <c r="H7" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2">
-        <v>3.07</v>
+        <v>3.14</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>6.14</v>
+        <v>12.56</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2">
-        <v>3.79</v>
+        <v>3.85</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>7.58</v>
+        <v>15.4</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="2">
-        <v>0</v>
+        <v>1.99</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="3"/>
+        <v>1.99</v>
+      </c>
+      <c r="F10" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
       <c r="H10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="I10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -1459,12 +1525,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -1480,21 +1546,21 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -1510,21 +1576,21 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -1540,21 +1606,21 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -1570,37 +1636,51 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
       <c r="C16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="F16" s="3">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
       <c r="H16" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="I16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -1619,23 +1699,34 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
       <c r="C18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="F18" s="3">
+        <v>55</v>
+      </c>
       <c r="H18" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="I18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="C19" s="3">
         <v>0</v>
       </c>
@@ -1643,7 +1734,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E19:E22" si="1">C19*D19</f>
         <v>0</v>
       </c>
       <c r="F19" s="3"/>
@@ -1651,23 +1742,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
+        <v>36.380000000000003</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="3"/>
+        <f t="shared" si="1"/>
+        <v>36.380000000000003</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
       <c r="H20" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="C21" s="3">
         <v>0</v>
       </c>
@@ -1675,7 +1771,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F21" s="3"/>
@@ -1683,36 +1779,99 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:9">
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="H22" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" ref="E23:E24" si="2">C23*D23</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="H23" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="H24" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="H25" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="1" customFormat="1">
+      <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="6">
-        <f>SUM(E2:E21)</f>
-        <v>451.46</v>
-      </c>
-      <c r="F22" s="7">
-        <f>SUM(F2:F21)</f>
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F23" s="7">
-        <f>1500-F22</f>
-        <v>95</v>
-      </c>
-      <c r="I23" t="s">
-        <v>23</v>
+      <c r="E26" s="6">
+        <f>SUM(E2:E25)</f>
+        <v>497.35</v>
+      </c>
+      <c r="F26" s="7">
+        <f>SUM(F2:F25)</f>
+        <v>1498.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="F27" s="7">
+        <f>1500-F26</f>
+        <v>1.4000000000000909</v>
+      </c>
+      <c r="I27" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B8" r:id="rId3" display="http://www.hobbyking.com/hobbyking/store/__22447__Slow_Fly_Electric_Prop_1045R_SF_RH_Rotation_4_pc_.html"/>
-    <hyperlink ref="B17" r:id="rId4" display="http://www.hobbyking.com/hobbyking/store/uh_viewItem.asp?idProduct=2169"/>
-    <hyperlink ref="B9" r:id="rId5" display="http://www.hobbyking.com/hobbyking/store/__22451__Slow_Fly_Electric_Prop_11x4_7SF_RH_Rotation_4_pc_.html"/>
+    <hyperlink ref="B8" r:id="rId2" display="http://www.hobbyking.com/hobbyking/store/__22447__Slow_Fly_Electric_Prop_1045R_SF_RH_Rotation_4_pc_.html"/>
+    <hyperlink ref="B17" r:id="rId3" display="http://www.hobbyking.com/hobbyking/store/uh_viewItem.asp?idProduct=2169"/>
+    <hyperlink ref="B9" r:id="rId4" display="http://www.hobbyking.com/hobbyking/store/__22451__Slow_Fly_Electric_Prop_11x4_7SF_RH_Rotation_4_pc_.html"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1732,56 +1891,56 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="51" customHeight="1" thickBot="1">
       <c r="A1" s="12"/>
       <c r="B1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="N1" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="15" t="s">
+    </row>
+    <row r="2" spans="1:14" ht="17.25" customHeight="1">
+      <c r="A2" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>58</v>
       </c>
       <c r="B2" s="18">
         <v>9.56</v>
@@ -1823,9 +1982,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="17.25" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="21">
         <v>12.42</v>
@@ -1867,9 +2026,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="17.25" customHeight="1">
       <c r="A4" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="25">
         <v>14.26</v>
@@ -1909,9 +2068,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="17.25" customHeight="1">
       <c r="A5" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="25">
         <v>14.26</v>
@@ -1953,9 +2112,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="17.25" customHeight="1">
       <c r="A6" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" s="25">
         <v>18.68</v>
@@ -1997,9 +2156,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="17.25" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="25">
         <v>14.99</v>
@@ -2039,9 +2198,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="17.25" customHeight="1" thickBot="1">
       <c r="A8" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" s="29">
         <v>12.22</v>
@@ -2083,127 +2242,127 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
+    <row r="10" spans="1:14" ht="17.25" customHeight="1" thickBot="1"/>
+    <row r="11" spans="1:14" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A11" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="54"/>
+    </row>
+    <row r="12" spans="1:14" ht="17.25" customHeight="1">
+      <c r="A12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="32">
+        <v>12.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="29" thickBot="1">
+      <c r="A13" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="34">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="17.25" customHeight="1" thickBot="1"/>
+    <row r="16" spans="1:14" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A16" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="54"/>
-    </row>
-    <row r="12" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="B16" s="13" t="s">
         <v>43</v>
-      </c>
-      <c r="B12" s="33">
-        <v>12.95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="35">
-        <v>6.95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>45</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A17" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="B17" s="36">
+        <v>3.02</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="39"/>
+    </row>
+    <row r="18" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A18" s="40" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+      <c r="B18" s="41">
+        <v>2.69</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="44"/>
+    </row>
+    <row r="19" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A19" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="37">
-        <v>3.02</v>
-      </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="40"/>
-    </row>
-    <row r="18" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="B19" s="41">
+        <v>3.36</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="44"/>
+    </row>
+    <row r="20" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="45">
+        <v>3.07</v>
+      </c>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46">
+        <v>9.5</v>
+      </c>
+      <c r="F20" s="47">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A21" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="42">
-        <v>2.69</v>
-      </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="45"/>
-    </row>
-    <row r="19" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+      <c r="B21" s="41">
+        <v>3.48</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43">
+        <v>11</v>
+      </c>
+      <c r="F21" s="49">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A22" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="42">
-        <v>3.36</v>
-      </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="45"/>
-    </row>
-    <row r="20" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="46">
-        <v>3.07</v>
-      </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47">
-        <v>9.5</v>
-      </c>
-      <c r="F20" s="48">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="42">
-        <v>3.48</v>
-      </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44">
-        <v>11</v>
-      </c>
-      <c r="F21" s="50">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="52">
+      <c r="B22" s="51">
         <v>3.79</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53">
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52">
         <v>12</v>
       </c>
-      <c r="F22" s="35">
+      <c r="F22" s="34">
         <v>131</v>
       </c>
     </row>
@@ -2227,5 +2386,10 @@
     <hyperlink ref="A21" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to TX/RX Parts
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
   <si>
     <t>Part</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Turnigy nano-Tech 5000mAh 3S 35C</t>
   </si>
   <si>
-    <t>Transmitter RF Module</t>
-  </si>
-  <si>
     <t>Transmitter Battery</t>
   </si>
   <si>
@@ -119,21 +116,6 @@
   </si>
   <si>
     <t>http://www.hobbyking.com/hobbyking/store/__31544__Turnigy_9XR_Transmitter_Mode_2_No_Module_.html</t>
-  </si>
-  <si>
-    <t>OrangeRX DSMX/DSM2 2.4GHz Module</t>
-  </si>
-  <si>
-    <t>http://www.hobbyking.com/hobbyking/store/__24656__OrangeRX_DSMX_DSM2_2_4Ghz_Transmitter_Module_JR_Turnigy_compatible_.html</t>
-  </si>
-  <si>
-    <t>Receiver</t>
-  </si>
-  <si>
-    <t>Orange DSM2 2.4Ghz 9CH</t>
-  </si>
-  <si>
-    <t>http://www.hobbyking.com/hobbyking/store/uh_viewItem.asp?idProduct=17621</t>
   </si>
   <si>
     <t>Turnigy 2650mAh 3S 1C</t>
@@ -286,6 +268,33 @@
   </si>
   <si>
     <t>Telemetry Radio</t>
+  </si>
+  <si>
+    <t>Transmitter RF Module/RX</t>
+  </si>
+  <si>
+    <t>FrSky DJT 2.4Ghz Combo Pack for JR w/ Telemetry Module &amp; V8FR-II RX</t>
+  </si>
+  <si>
+    <t>http://www.hobbyking.com/hobbyking/store/%5F%5F14349%5F%5FFrSky%5FDJT%5F2%5F4Ghz%5FCombo%5FPack%5Ffor%5FJR%5Fw%5FTelemetry%5FModule%5FV8FR%5FII%5FRX.html</t>
+  </si>
+  <si>
+    <t>Transmitter Antenna</t>
+  </si>
+  <si>
+    <t>Transmitter Case</t>
+  </si>
+  <si>
+    <t>2.4Ghz 7DB Antenna for FrSky Modules (And compatible Radios/Modules)</t>
+  </si>
+  <si>
+    <t>http://www.hobbyking.com/hobbyking/store/%5F%5F20108%5F%5F2%5F4Ghz%5F7DB%5FAntenna%5Ffor%5FFrSky%5FModules%5FAnd%5Fcompatible%5FRadios%5FModules%5F.html</t>
+  </si>
+  <si>
+    <t>Turnigy 9XR Aluminum Carrying Case</t>
+  </si>
+  <si>
+    <t>http://www.hobbyking.com/hobbyking/store/%5F%5F26019%5F%5FTurnigy%5F9XR%5FAluminum%5FCarrying%5FCase.html</t>
   </si>
 </sst>
 </file>
@@ -739,7 +748,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -755,8 +764,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -856,8 +866,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -868,6 +879,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1206,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1277,7 +1289,7 @@
         <v>25</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1297,7 +1309,7 @@
         <v>89</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E25" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E28" si="0">C3*D3</f>
         <v>89</v>
       </c>
       <c r="F3" s="3">
@@ -1307,7 +1319,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I3" t="s">
         <v>23</v>
@@ -1318,7 +1330,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C4" s="3">
         <v>6</v>
@@ -1338,7 +1350,7 @@
         <v>25</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1390,7 +1402,7 @@
         <v>25</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I6" t="s">
         <v>26</v>
@@ -1398,10 +1410,10 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -1420,10 +1432,10 @@
         <v>25</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1431,7 +1443,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C8" s="3">
         <v>4</v>
@@ -1448,7 +1460,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1456,7 +1468,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C9" s="3">
         <v>4</v>
@@ -1473,7 +1485,7 @@
         <v>25</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1481,7 +1493,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -1500,10 +1512,10 @@
         <v>25</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1526,51 +1538,28 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2">
-        <v>49.99</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="0"/>
-        <v>49.99</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
       <c r="D13" s="2">
-        <v>29.99</v>
+        <v>49.95</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>29.99</v>
+        <v>49.95</v>
       </c>
       <c r="F13" s="3">
         <v>0</v>
@@ -1582,28 +1571,28 @@
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
       <c r="D14" s="2">
-        <v>12.79</v>
+        <v>38.33</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>12.79</v>
+        <v>38.33</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G14" t="s">
         <v>25</v>
@@ -1611,29 +1600,29 @@
       <c r="H14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I14" t="s">
-        <v>39</v>
+      <c r="I14" s="55" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="2">
-        <v>24.95</v>
+        <v>12.79</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>24.95</v>
+        <v>12.79</v>
       </c>
       <c r="F15" s="3">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G15" t="s">
         <v>25</v>
@@ -1642,141 +1631,155 @@
         <v>9</v>
       </c>
       <c r="I15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" t="s">
         <v>84</v>
-      </c>
-      <c r="B16" t="s">
-        <v>81</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" s="2">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" ref="E16" si="1">C16*D16</f>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>12.99</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>12.99</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
         <v>49</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E19" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F19" s="3">
         <v>10</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G19" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="3">
+      <c r="H19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D20" s="2">
         <v>6.95</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
         <v>6.95</v>
       </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4" t="s">
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="3">
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="3">
         <v>1</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D21" s="2">
         <v>16</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F21" s="3">
         <v>55</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" ref="E19:E22" si="1">C19*D19</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="H19" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2">
-        <v>36.380000000000003</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="1"/>
-        <v>36.380000000000003</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="3"/>
       <c r="H21" s="4" t="s">
-        <v>9</v>
+        <v>66</v>
+      </c>
+      <c r="I21" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1787,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E22:E25" si="2">C22*D22</f>
         <v>0</v>
       </c>
       <c r="F22" s="3"/>
@@ -1796,19 +1799,24 @@
       </c>
     </row>
     <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
       <c r="C23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2">
-        <v>0</v>
+        <v>36.380000000000003</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" ref="E23:E24" si="2">C23*D23</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="3"/>
+        <f t="shared" si="2"/>
+        <v>36.380000000000003</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
       <c r="H23" s="4" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1835,7 +1843,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F25" s="3"/>
@@ -1843,25 +1851,73 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:9">
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" ref="E26:E27" si="3">C26*D26</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="H26" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="H27" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="H28" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="1" customFormat="1">
+      <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="6">
-        <f>SUM(E2:E25)</f>
-        <v>497.35</v>
-      </c>
-      <c r="F26" s="7">
-        <f>SUM(F2:F25)</f>
-        <v>1498.6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="F27" s="7">
-        <f>1500-F26</f>
-        <v>1.4000000000000909</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="E29" s="6">
+        <f>SUM(E2:E28)</f>
+        <v>502.64</v>
+      </c>
+      <c r="F29" s="7">
+        <f>SUM(F2:F28)</f>
+        <v>1493.8999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="F30" s="7">
+        <f>1500-F29</f>
+        <v>6.1000000000001364</v>
+      </c>
+      <c r="I30" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1870,8 +1926,9 @@
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
     <hyperlink ref="B8" r:id="rId2" display="http://www.hobbyking.com/hobbyking/store/__22447__Slow_Fly_Electric_Prop_1045R_SF_RH_Rotation_4_pc_.html"/>
-    <hyperlink ref="B17" r:id="rId3" display="http://www.hobbyking.com/hobbyking/store/uh_viewItem.asp?idProduct=2169"/>
+    <hyperlink ref="B20" r:id="rId3" display="http://www.hobbyking.com/hobbyking/store/uh_viewItem.asp?idProduct=2169"/>
     <hyperlink ref="B9" r:id="rId4" display="http://www.hobbyking.com/hobbyking/store/__22451__Slow_Fly_Electric_Prop_11x4_7SF_RH_Rotation_4_pc_.html"/>
+    <hyperlink ref="I14" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1899,48 +1956,48 @@
     <row r="1" spans="1:14" ht="51" customHeight="1" thickBot="1">
       <c r="A1" s="12"/>
       <c r="B1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="I1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="N1" s="16" t="s">
         <v>49</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="17.25" customHeight="1">
       <c r="A2" s="17" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B2" s="18">
         <v>9.56</v>
@@ -1984,7 +2041,7 @@
     </row>
     <row r="3" spans="1:14" ht="17.25" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B3" s="21">
         <v>12.42</v>
@@ -2028,7 +2085,7 @@
     </row>
     <row r="4" spans="1:14" ht="17.25" customHeight="1">
       <c r="A4" s="24" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B4" s="25">
         <v>14.26</v>
@@ -2070,7 +2127,7 @@
     </row>
     <row r="5" spans="1:14" ht="17.25" customHeight="1">
       <c r="A5" s="24" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B5" s="25">
         <v>14.26</v>
@@ -2114,7 +2171,7 @@
     </row>
     <row r="6" spans="1:14" ht="17.25" customHeight="1">
       <c r="A6" s="24" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B6" s="25">
         <v>18.68</v>
@@ -2158,7 +2215,7 @@
     </row>
     <row r="7" spans="1:14" ht="17.25" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B7" s="25">
         <v>14.99</v>
@@ -2200,7 +2257,7 @@
     </row>
     <row r="8" spans="1:14" ht="17.25" customHeight="1" thickBot="1">
       <c r="A8" s="28" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B8" s="29">
         <v>12.22</v>
@@ -2245,13 +2302,13 @@
     <row r="10" spans="1:14" ht="17.25" customHeight="1" thickBot="1"/>
     <row r="11" spans="1:14" ht="17.25" customHeight="1" thickBot="1">
       <c r="A11" s="53" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B11" s="54"/>
     </row>
     <row r="12" spans="1:14" ht="17.25" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B12" s="32">
         <v>12.95</v>
@@ -2259,7 +2316,7 @@
     </row>
     <row r="13" spans="1:14" ht="29" thickBot="1">
       <c r="A13" s="33" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B13" s="34">
         <v>6.95</v>
@@ -2268,23 +2325,23 @@
     <row r="15" spans="1:14" ht="17.25" customHeight="1" thickBot="1"/>
     <row r="16" spans="1:14" ht="17.25" customHeight="1" thickBot="1">
       <c r="A16" s="13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17.25" customHeight="1">
       <c r="A17" s="35" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B17" s="36">
         <v>3.02</v>
@@ -2296,7 +2353,7 @@
     </row>
     <row r="18" spans="1:6" ht="17.25" customHeight="1">
       <c r="A18" s="40" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B18" s="41">
         <v>2.69</v>
@@ -2308,7 +2365,7 @@
     </row>
     <row r="19" spans="1:6" ht="17.25" customHeight="1">
       <c r="A19" s="40" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B19" s="41">
         <v>3.36</v>
@@ -2320,7 +2377,7 @@
     </row>
     <row r="20" spans="1:6" ht="17.25" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B20" s="45">
         <v>3.07</v>
@@ -2336,7 +2393,7 @@
     </row>
     <row r="21" spans="1:6" ht="17.25" customHeight="1">
       <c r="A21" s="48" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B21" s="41">
         <v>3.48</v>
@@ -2352,7 +2409,7 @@
     </row>
     <row r="22" spans="1:6" ht="17.25" customHeight="1" thickBot="1">
       <c r="A22" s="50" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B22" s="51">
         <v>3.79</v>

</xml_diff>